<commit_message>
Hibernate Spring Java Configuration
</commit_message>
<xml_diff>
--- a/arun_error-and-solutions .xlsx
+++ b/arun_error-and-solutions .xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>S.No</t>
   </si>
@@ -90,6 +90,18 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>27.Oct.2016</t>
+  </si>
+  <si>
+    <t>Connect Spring Hibernate Application with Oracle</t>
+  </si>
+  <si>
+    <t>http://o7planning.org/en/10305/simple-login-java-web-application-using-spring-mvc-spring-security-and-spring-jdbc                                                                                                                https://community.oracle.com/thread/2278282</t>
+  </si>
+  <si>
+    <t>1 Hours</t>
   </si>
 </sst>
 </file>
@@ -526,7 +538,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -537,7 +549,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -604,12 +616,22 @@
     </row>
     <row r="3" spans="1:8" ht="45.75" customHeight="1">
       <c r="A3" s="18"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="18"/>
+      <c r="B3" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>21</v>
+      </c>
       <c r="H3" s="18"/>
     </row>
     <row r="4" spans="1:8" ht="45.75" customHeight="1">
@@ -696,9 +718,10 @@
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1"/>
     <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="E3" r:id="rId3" display="https://community.oracle.com/thread/2278282"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Getting Data Through Rest Controller in Angular without Service
</commit_message>
<xml_diff>
--- a/arun_error-and-solutions .xlsx
+++ b/arun_error-and-solutions .xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="19320" windowHeight="6330"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="19320" windowHeight="6330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DAY_01" sheetId="4" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>S.No</t>
   </si>
@@ -102,6 +102,30 @@
   </si>
   <si>
     <t>1 Hours</t>
+  </si>
+  <si>
+    <t>09.Nov.2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://spring.io/guides/gs/rest-service-cors/                                                                                              https://spring.io/guides/gs/consuming-rest-angularjs/                                                                       </t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>1 Hour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creating Rest Controller using CORS and access in angular </t>
+  </si>
+  <si>
+    <t>XMLHttpRequest cannot load http://localhost:8989/arun_online_collaboration/blog/allblogs. No 'Access-Control-Allow-Origin' header is present on the requested resource. Origin 'http://127.0.0.1:8887' is therefore not allowed access.</t>
+  </si>
+  <si>
+    <t>Handler method must be annoted with  @CrossOrigin(origins="http://127.0.0.1:8887") and pass the origin (your server where's your second application is running)</t>
+  </si>
+  <si>
+    <t>https://spring.io/guides/gs/rest-service-cors/</t>
   </si>
 </sst>
 </file>
@@ -538,7 +562,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -548,20 +572,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="31.125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23.25" style="1" customWidth="1"/>
-    <col min="5" max="5" width="67.25" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.75" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="20.75" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="31.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="67.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="45">
@@ -646,13 +670,25 @@
     </row>
     <row r="5" spans="1:8" s="12" customFormat="1" ht="42.75" customHeight="1">
       <c r="A5" s="18"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="14"/>
+      <c r="B5" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>30</v>
+      </c>
       <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
+      <c r="E5" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="18">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:8" s="12" customFormat="1">
       <c r="A6" s="18"/>
@@ -719,9 +755,10 @@
     <hyperlink ref="E2" r:id="rId1"/>
     <hyperlink ref="D2" r:id="rId2"/>
     <hyperlink ref="E3" r:id="rId3" display="https://community.oracle.com/thread/2278282"/>
+    <hyperlink ref="E5" r:id="rId4" display="https://spring.io/guides/gs/consuming-rest-angularjs/                                                                       "/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -729,15 +766,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="98" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.125" customWidth="1"/>
-    <col min="2" max="2" width="73.25" customWidth="1"/>
-    <col min="3" max="3" width="52.25" customWidth="1"/>
-    <col min="4" max="4" width="56.375" customWidth="1"/>
-    <col min="5" max="10" width="9.125" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
+    <col min="2" max="2" width="73.28515625" customWidth="1"/>
+    <col min="3" max="3" width="52.28515625" customWidth="1"/>
+    <col min="4" max="4" width="56.42578125" customWidth="1"/>
+    <col min="5" max="10" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -755,10 +794,18 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="45.75" customHeight="1">
-      <c r="A2" s="3"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="10"/>
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="3"/>
@@ -808,8 +855,11 @@
       <c r="D12" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -821,10 +871,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="45.875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="41.875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="46.625" customWidth="1"/>
-    <col min="5" max="5" width="65.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="41.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="46.5703125" customWidth="1"/>
+    <col min="5" max="5" width="65.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="45" customHeight="1">

</xml_diff>

<commit_message>
Crud Done 17 Nov
</commit_message>
<xml_diff>
--- a/arun_error-and-solutions .xlsx
+++ b/arun_error-and-solutions .xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="47">
   <si>
     <t>S.No</t>
   </si>
@@ -126,6 +126,46 @@
   </si>
   <si>
     <t>https://spring.io/guides/gs/rest-service-cors/</t>
+  </si>
+  <si>
+    <t>12.Nov.2016</t>
+  </si>
+  <si>
+    <t>Getting the current user Details</t>
+  </si>
+  <si>
+    <t>http://docs.spring.io/spring-security/site/docs/4.0.2.RELEASE/reference/htmlsingle/#obtaining-information-about-the-current-user</t>
+  </si>
+  <si>
+    <t>13.Nov.2016</t>
+  </si>
+  <si>
+    <t>Crud with angular + Spring MVC</t>
+  </si>
+  <si>
+    <t>http://websystique.com/springmvc/spring-4-mvc-angularjs-crud-application-using-ngresource/</t>
+  </si>
+  <si>
+    <t>14.Nov.2016</t>
+  </si>
+  <si>
+    <t>Add Spring Security Filter in webInitialize (java based web.xml)</t>
+  </si>
+  <si>
+    <t>http://stackoverflow.com/questions/14205140/spring-security-without-web-xml?answertab=votes#tab-top</t>
+  </si>
+  <si>
+    <t>10 mnts</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>Spring Security was not working and their was no error</t>
+  </si>
+  <si>
+    <t>container.addFilter("springSecurityFilterChain", new DelegatingFilterProxy("springSecurityFilterChain"))
+                    .addMappingForUrlPatterns(null, false, "/*");</t>
   </si>
 </sst>
 </file>
@@ -562,7 +602,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -572,8 +612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="A5" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -700,35 +740,59 @@
       <c r="G6" s="18"/>
       <c r="H6" s="18"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" ht="45">
       <c r="A7" s="18"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="14"/>
+      <c r="B7" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>35</v>
+      </c>
       <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
+      <c r="E7" s="9" t="s">
+        <v>36</v>
+      </c>
       <c r="F7" s="14"/>
       <c r="G7" s="18"/>
       <c r="H7" s="18"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" ht="30">
       <c r="A8" s="18"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="14"/>
+      <c r="B8" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>38</v>
+      </c>
       <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
+      <c r="E8" s="9" t="s">
+        <v>39</v>
+      </c>
       <c r="F8" s="14"/>
       <c r="G8" s="18"/>
       <c r="H8" s="18"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" ht="45">
       <c r="A9" s="18"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="14"/>
+      <c r="B9" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>41</v>
+      </c>
       <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
+      <c r="E9" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" s="18">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="18"/>
@@ -756,9 +820,12 @@
     <hyperlink ref="D2" r:id="rId2"/>
     <hyperlink ref="E3" r:id="rId3" display="https://community.oracle.com/thread/2278282"/>
     <hyperlink ref="E5" r:id="rId4" display="https://spring.io/guides/gs/consuming-rest-angularjs/                                                                       "/>
+    <hyperlink ref="E7" r:id="rId5" location="obtaining-information-about-the-current-user"/>
+    <hyperlink ref="E8" r:id="rId6"/>
+    <hyperlink ref="E9" r:id="rId7" location="tab-top"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -766,8 +833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -807,11 +874,19 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="3"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="10"/>
+    <row r="3" spans="1:4" ht="45">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="4" spans="1:4" ht="45.75" customHeight="1">
       <c r="A4" s="13"/>
@@ -857,9 +932,10 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2" location="tab-top"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>